<commit_message>
#3291 add email to case, contact, event participant detailed & custom exports
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
@@ -525,7 +525,7 @@
     <t>SORMAS Version</t>
   </si>
   <si>
-    <t>${project.version}</t>
+    <t>1.51.0-SNAPSHOT</t>
   </si>
 </sst>
 </file>
@@ -6929,8 +6929,8 @@
       <c r="E76" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F76" s="2" t="s">
-        <v>40</v>
+      <c r="F76" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>40</v>
@@ -9828,14 +9828,14 @@
       <c r="C111" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D111" s="2" t="s">
-        <v>40</v>
+      <c r="D111" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F111" s="2" t="s">
-        <v>40</v>
+      <c r="F111" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="G111" s="2" t="s">
         <v>40</v>
@@ -9917,8 +9917,8 @@
       <c r="E112" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F112" s="2" t="s">
-        <v>40</v>
+      <c r="F112" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="G112" s="2" t="s">
         <v>40</v>
@@ -11494,8 +11494,8 @@
       <c r="E131" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F131" s="2" t="s">
-        <v>40</v>
+      <c r="F131" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="G131" s="1" t="s">
         <v>39</v>

</xml_diff>